<commit_message>
random number function - created separate class - FunctionUtils.java and also added log4j dependency in pom.xml
</commit_message>
<xml_diff>
--- a/testdata/Login.xlsx
+++ b/testdata/Login.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sameer\Title21Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6285" windowHeight="5835" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="5835" windowWidth="6285" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="GroupDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
+    <sheet name="GroupDetails" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -58,6 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,17 +101,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -127,10 +128,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -165,7 +166,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,7 +201,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,21 +295,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -325,7 +326,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -377,15 +378,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -393,17 +394,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -444,13 +445,13 @@
       <c r="C5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
@@ -458,8 +459,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -479,6 +480,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated testcase and POM file.
</commit_message>
<xml_diff>
--- a/testdata/Login.xlsx
+++ b/testdata/Login.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sameer\Title21Automation\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neosoft\git\Title21Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="5835" windowWidth="6285" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" windowHeight="6060" windowWidth="19380" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
@@ -51,7 +51,7 @@
     <t>Dallas</t>
   </si>
   <si>
-    <t>Test7890</t>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,14 +454,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.0" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
add employee Test case.
</commit_message>
<xml_diff>
--- a/testdata/Login.xlsx
+++ b/testdata/Login.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sameer\Title21Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="5835" windowWidth="6285" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6285" windowHeight="5835" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
-    <sheet name="GroupDetails" r:id="rId2" sheetId="2"/>
+    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="GroupDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateEmployee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>sysadmin</t>
   </si>
@@ -52,17 +53,87 @@
   </si>
   <si>
     <t>Test7890</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>employeeID</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>businessUnit</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>45, GB Thosmson Road</t>
+  </si>
+  <si>
+    <t>Alex Starch</t>
+  </si>
+  <si>
+    <t>NewyorkCity</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>alexstarch@testmail.com</t>
+  </si>
+  <si>
+    <t>866-782-4964</t>
+  </si>
+  <si>
+    <t>John Smith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,18 +171,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -128,10 +208,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -166,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,7 +281,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,21 +375,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -326,7 +406,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -378,15 +458,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -394,17 +474,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -445,22 +525,22 @@
       <c r="C5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -480,6 +560,193 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4567</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3">
+        <v>10019</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4567</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3">
+        <v>10019</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4567</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="3">
+        <v>10019</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1"/>
+    <hyperlink ref="M3" r:id="rId2"/>
+    <hyperlink ref="M4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>